<commit_message>
Automation spreed sheet project
</commit_message>
<xml_diff>
--- a/transaction.xlsx
+++ b/transaction.xlsx
@@ -1,70 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e3226fd1996d480/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{07C4D00F-C1A7-4AF4-8938-B51747CA34DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D56208F4-B621-4017-BBFE-3725DDA7E068}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4EA4B221-5244-482C-BC09-24514E457317}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>transaction_id</t>
-  </si>
-  <si>
-    <t>product_id</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -82,24 +47,286 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <layout/>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <val>
+            <numRef>
+              <f>Sheet1!$E$2:$E$5</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="4"/>
+                <pt idx="0">
+                  <v>4.5</v>
+                </pt>
+                <pt idx="1">
+                  <v>5.4</v>
+                </pt>
+                <pt idx="2">
+                  <v>7.65</v>
+                </pt>
+                <pt idx="3">
+                  <v>9.675000000000001</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <crossAx val="100"/>
+        <crosses val="autoZero"/>
+        <auto val="0"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <crossAx val="10"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="between"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+      <overlay val="0"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$E$2:$E$5</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -398,87 +625,110 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E6A00F0-BE8C-49E1-A27C-AEDA893834CE}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col width="13.7109375" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="10.5703125" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>transaction_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>product_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1002</v>
+      </c>
+      <c r="B3" t="n">
         <v>2</v>
       </c>
+      <c r="C3" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5.4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1001</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>5.95</v>
-      </c>
-      <c r="D2">
-        <v>6</v>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E4" t="n">
+        <v>7.65</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1002</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>6.95</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1003</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5">
+      <c r="A5" t="n">
         <v>1004</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
-        <v>10.75</v>
-      </c>
-      <c r="D5">
+      <c r="C5" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="D5" t="n">
         <v>11</v>
+      </c>
+      <c r="E5" t="n">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>